<commit_message>
feat(CMPF-1037) JXLS 모듈 의존성 제거
</commit_message>
<xml_diff>
--- a/modules/core/excel-generator/src/test/resources/templates/template.xlsx
+++ b/modules/core/excel-generator/src/test/resources/templates/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyh/dev/mylib/kotlin/kotlin-common-library/modules/core/excel-generator/src/test/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB291D27-8D17-C440-B5C5-12F951B0E5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB66B532-AEC5-D54E-8B11-B7A099D8FA24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="4740" windowWidth="35440" windowHeight="27520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3400" yWindow="4740" windowWidth="35440" windowHeight="27520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report(세로)" sheetId="1" r:id="rId1"/>
@@ -2814,7 +2814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3C7E00-1A54-7244-AD9C-884797BC931B}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -2919,8 +2919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA2B50C-AA25-8B49-B0CA-84B6326704E6}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>

</xml_diff>

<commit_message>
feat(CMPF-1037) floatimage 마커 추가
</commit_message>
<xml_diff>
--- a/modules/core/excel-generator/src/test/resources/templates/template.xlsx
+++ b/modules/core/excel-generator/src/test/resources/templates/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyh/dev/mylib/kotlin/kotlin-common-library/modules/core/excel-generator/src/test/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB66B532-AEC5-D54E-8B11-B7A099D8FA24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A000544-7384-4A4B-9E3D-48E167D56C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="4740" windowWidth="35440" windowHeight="27520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="600" windowWidth="35440" windowHeight="27520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report(세로)" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="106" r:id="rId4"/>
+    <pivotCache cacheId="136" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
     <t>${title}</t>
   </si>
@@ -130,6 +130,30 @@
   </si>
   <si>
     <t>개수 : 이름</t>
+  </si>
+  <si>
+    <t>${floatimage(ci, "", 0:-1)}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${floatimage(ci, "", -1:-1)}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${floatimage(logo, "", 0:-0)}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${floatimage(ci, "", 0:0)}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${floatimage(ci, B11, 0:-1)}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${floatimage(ci, C10, 0:-1)}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2090,49 +2114,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7D345E0-1F9E-3542-9E98-DBF333DED568}" name="피벗 테이블2" cacheId="106" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="M6:N8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="개수 : 이름" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B913C3A8-83B3-D24B-8F4B-0985F48AA6EC}" name="피벗 테이블3" cacheId="106" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" grandTotalCaption="총" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="직급">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B913C3A8-83B3-D24B-8F4B-0985F48AA6EC}" name="피벗 테이블3" cacheId="136" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" grandTotalCaption="총" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="직급">
   <location ref="I6:K8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
@@ -2317,6 +2299,48 @@
       </pivotArea>
     </chartFormat>
   </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7D345E0-1F9E-3542-9E98-DBF333DED568}" name="피벗 테이블2" cacheId="136" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="M6:N8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="개수 : 이름" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -2646,10 +2670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -2722,6 +2746,9 @@
         <v>7</v>
       </c>
       <c r="D6" s="5"/>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
       <c r="I6" s="15" t="s">
         <v>4</v>
       </c>
@@ -2785,6 +2812,11 @@
       <c r="B9">
         <f>SUM(C6)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="B10" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2812,10 +2844,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3C7E00-1A54-7244-AD9C-884797BC931B}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -2885,6 +2917,9 @@
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
       <c r="F7">
         <f>SUM(B7)</f>
         <v>0</v>
@@ -2898,11 +2933,49 @@
         <v>9</v>
       </c>
     </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="21"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B23:C27"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2919,8 +2992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA2B50C-AA25-8B49-B0CA-84B6326704E6}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>

</xml_diff>

<commit_message>
feat(CMPF-1037) floatimage와 image 마커 통합. Named range 지원
</commit_message>
<xml_diff>
--- a/modules/core/excel-generator/src/test/resources/templates/template.xlsx
+++ b/modules/core/excel-generator/src/test/resources/templates/template.xlsx
@@ -2,24 +2,28 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyh/dev/mylib/kotlin/kotlin-common-library/modules/core/excel-generator/src/test/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A000544-7384-4A4B-9E3D-48E167D56C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7B55F2-8CAC-914E-83E0-8AB1D71C4CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="600" windowWidth="35440" windowHeight="27520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="600" windowWidth="35440" windowHeight="27520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report(세로)" sheetId="1" r:id="rId1"/>
     <sheet name="Report (가로)" sheetId="2" r:id="rId2"/>
     <sheet name="Report(셀병합)" sheetId="3" r:id="rId3"/>
+    <sheet name="Report(Named Range)" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="employeeList">'Report(Named Range)'!$A$6:$C$6</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="136" r:id="rId4"/>
+    <pivotCache cacheId="302" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
   <si>
     <t>${title}</t>
   </si>
@@ -132,27 +136,39 @@
     <t>개수 : 이름</t>
   </si>
   <si>
-    <t>${floatimage(ci, "", 0:-1)}</t>
+    <t>${image(ci, C10, 0:-1)}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>${floatimage(ci, "", -1:-1)}</t>
+    <t>${image(ci, B11, 0:-1)}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>${floatimage(logo, "", 0:-0)}</t>
+    <t>${image(ci, "", 0:-1)}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>${floatimage(ci, "", 0:0)}</t>
+    <t>${image(logo, "", 0:-0)}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>${floatimage(ci, B11, 0:-1)}</t>
+    <t>${image(ci, "", 0:0)}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>${floatimage(ci, C10, 0:-1)}</t>
+    <t>${image(ci, "", -1:-1)}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${image.logo}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${image(ci)}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${repeat(collection=employees, range=employeeList, var=emp)}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -354,7 +370,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -411,9 +427,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -435,13 +448,327 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="좋음" xfId="1" builtinId="26"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="하이퍼링크" xfId="2" builtinId="8"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="93">
+    <dxf>
+      <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="#,##0_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <charset val="129"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <charset val="129"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="double"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="#,##0_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <charset val="129"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <charset val="129"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="double"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="#,##0_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <charset val="129"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <charset val="129"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="double"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="#,##0_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <charset val="129"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <charset val="129"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="double"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="#,##0_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <charset val="129"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <charset val="129"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="double"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2114,7 +2441,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B913C3A8-83B3-D24B-8F4B-0985F48AA6EC}" name="피벗 테이블3" cacheId="136" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" grandTotalCaption="총" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="직급">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B913C3A8-83B3-D24B-8F4B-0985F48AA6EC}" name="피벗 테이블3" cacheId="302" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" grandTotalCaption="총" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10" rowHeaderCaption="직급">
   <location ref="I6:K8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
@@ -2158,17 +2485,17 @@
     <dataField name="평균 급여" fld="2" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="15">
-    <format dxfId="16">
+    <format dxfId="92">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="91">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="90">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -2178,7 +2505,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="89">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -2188,7 +2515,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="88">
       <pivotArea field="1" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2197,7 +2524,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="87">
       <pivotArea field="1" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -2206,23 +2533,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="86">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="7">
+    <format dxfId="83">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -2232,28 +2559,28 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
@@ -2261,7 +2588,7 @@
       </pivotArea>
     </format>
   </formats>
-  <chartFormats count="4">
+  <chartFormats count="6">
     <chartFormat chart="0" format="4" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -2298,6 +2625,24 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="9" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -2312,7 +2657,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7D345E0-1F9E-3542-9E98-DBF333DED568}" name="피벗 테이블2" cacheId="136" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7D345E0-1F9E-3542-9E98-DBF333DED568}" name="피벗 테이블2" cacheId="302" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="M6:N8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
@@ -2672,8 +3017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -2689,29 +3034,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="50" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="20"/>
       <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="24" t="str">
+      <c r="F1" s="23" t="str">
         <f>HYPERLINK("${url}", "${linkText}")</f>
         <v>${linkText}</v>
       </c>
-      <c r="G1" s="24"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:14" ht="32" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
@@ -2747,7 +3092,7 @@
       </c>
       <c r="D6" s="5"/>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I6" s="15" t="s">
         <v>4</v>
@@ -2769,7 +3114,7 @@
       <c r="I7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J7" s="28">
         <v>0</v>
       </c>
       <c r="K7" s="17" t="e">
@@ -2778,7 +3123,7 @@
       <c r="M7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="27">
         <v>1</v>
       </c>
     </row>
@@ -2792,16 +3137,16 @@
       <c r="I8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="29">
         <v>0</v>
       </c>
-      <c r="K8" s="16" t="e">
+      <c r="K8" s="29" t="e">
         <v>#DIV/0!</v>
       </c>
       <c r="M8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="27">
         <v>1</v>
       </c>
     </row>
@@ -2816,7 +3161,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="B10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2828,7 +3173,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="77" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>6000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2847,7 +3192,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -2858,26 +3203,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="21" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="20"/>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="32" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
@@ -2918,7 +3263,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F7">
         <f>SUM(B7)</f>
@@ -2935,39 +3280,39 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="B20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="B23" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="21"/>
+      <c r="B23" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="20"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3004,24 +3349,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="50" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21"/>
+      <c r="D1" s="20"/>
       <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="32" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
@@ -3034,7 +3379,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -3043,14 +3388,14 @@
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="26"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="26" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -3059,7 +3404,7 @@
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="21"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="12" t="s">
         <v>7</v>
       </c>
@@ -3091,7 +3436,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B8">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="76" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>6000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3102,4 +3447,130 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3E7F18-D735-9A4E-BC9A-79E1426A1776}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" customWidth="1"/>
+    <col min="5" max="6" width="20" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="50" customHeight="1">
+      <c r="A1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="20"/>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="23" t="str">
+        <f>HYPERLINK("${url}", "${linkText}")</f>
+        <v>${linkText}</v>
+      </c>
+      <c r="G1" s="23"/>
+    </row>
+    <row r="2" spans="1:7" ht="32" customHeight="1">
+      <c r="A2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <f>SUM(C6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="cellIs" dxfId="75" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+      <formula>6000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{235B57F8-47F7-C648-87B5-9EAD463C6935}">
+      <formula1>"사원, 대리, 과장, 차장, 부장"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>